<commit_message>
Added Users module test cases
</commit_message>
<xml_diff>
--- a/test_case/users/users_module_test_cases.xlsx
+++ b/test_case/users/users_module_test_cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\test_case_ai_quizwhiz_zluck_com\test_case\users\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\test_case_ai_quizwhiz_zluck_com\test_case\users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F192BC-9152-4418-A377-B0DE07E646F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F43686B-C293-4DCA-92B8-C99D07BCAECC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>Password should be updated, and login with new password should work</t>
+  </si>
+  <si>
+    <t>USR-016</t>
   </si>
 </sst>
 </file>
@@ -665,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -889,7 +892,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
@@ -929,7 +932,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
@@ -969,7 +972,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
@@ -989,7 +992,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
@@ -1008,6 +1011,26 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>